<commit_message>
Experimentos realizados. Dan bastante fuera de lo permitido.
</commit_message>
<xml_diff>
--- a/JMeter/Experimentos.xlsx
+++ b/JMeter/Experimentos.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="3120" yWindow="460" windowWidth="22480" windowHeight="14180" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Exp1 - Entr 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Exp 2 - Entr 1 (1)" sheetId="2" r:id="rId2"/>
-    <sheet name="Exp 2 - Entr 1 (2)" sheetId="3" r:id="rId3"/>
-    <sheet name="Exp 2 - Entr 2" sheetId="4" r:id="rId4"/>
+    <sheet name="Exp1-Entr1" sheetId="1" r:id="rId1"/>
+    <sheet name="Exp2-Entr1(1)" sheetId="2" r:id="rId2"/>
+    <sheet name="Exp2-Entr1(2)" sheetId="3" r:id="rId3"/>
+    <sheet name="Exp2-Entr2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -251,7 +251,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -316,7 +315,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Exp1 - Entr 1'!$N$19:$N$31</c:f>
+              <c:f>'Exp1-Entr1'!$N$19:$N$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -364,7 +363,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Exp1 - Entr 1'!$O$19:$O$31</c:f>
+              <c:f>'Exp1-Entr1'!$O$19:$O$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -420,11 +419,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-837375488"/>
-        <c:axId val="-837381040"/>
+        <c:axId val="-893104848"/>
+        <c:axId val="-893108512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-837375488"/>
+        <c:axId val="-893104848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1200.0"/>
@@ -471,7 +470,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -538,12 +536,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-837381040"/>
+        <c:crossAx val="-893108512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-837381040"/>
+        <c:axId val="-893108512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1200.0"/>
@@ -591,7 +589,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -657,7 +654,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-837375488"/>
+        <c:crossAx val="-893104848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -811,7 +808,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Exp 2 - Entr 1 (1)'!$B$6:$B$18</c:f>
+              <c:f>'Exp2-Entr1(1)'!$B$6:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -859,7 +856,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Exp 2 - Entr 1 (1)'!$C$6:$C$18</c:f>
+              <c:f>'Exp2-Entr1(1)'!$C$6:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -915,11 +912,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-863687360"/>
-        <c:axId val="-892401872"/>
+        <c:axId val="-837760240"/>
+        <c:axId val="-837757120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-863687360"/>
+        <c:axId val="-837760240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1032,12 +1029,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-892401872"/>
+        <c:crossAx val="-837757120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-892401872"/>
+        <c:axId val="-837757120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1149,7 +1146,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-863687360"/>
+        <c:crossAx val="-837760240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1307,7 +1304,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Exp 2 - Entr 1 (1)'!$B$6:$B$18</c:f>
+              <c:f>'Exp2-Entr1(1)'!$B$6:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1355,7 +1352,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Exp 2 - Entr 1 (1)'!$D$6:$D$18</c:f>
+              <c:f>'Exp2-Entr1(1)'!$D$6:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1411,11 +1408,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-856561408"/>
-        <c:axId val="-856558288"/>
+        <c:axId val="-837165184"/>
+        <c:axId val="-892310176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-856561408"/>
+        <c:axId val="-837165184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1527,12 +1524,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-856558288"/>
+        <c:crossAx val="-892310176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-856558288"/>
+        <c:axId val="-892310176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1644,7 +1641,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-856561408"/>
+        <c:crossAx val="-837165184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1799,7 +1796,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Exp 2 - Entr 1 (1)'!$B$6:$B$18</c:f>
+              <c:f>'Exp2-Entr1(1)'!$B$6:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1847,7 +1844,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Exp 2 - Entr 1 (1)'!$E$6:$E$18</c:f>
+              <c:f>'Exp2-Entr1(1)'!$E$6:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1903,11 +1900,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-837424640"/>
-        <c:axId val="-837421520"/>
+        <c:axId val="-837440336"/>
+        <c:axId val="-837437216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-837424640"/>
+        <c:axId val="-837440336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2019,12 +2016,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-837421520"/>
+        <c:crossAx val="-837437216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-837421520"/>
+        <c:axId val="-837437216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2136,7 +2133,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-837424640"/>
+        <c:crossAx val="-837440336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2225,7 +2222,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2266,7 +2262,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Exp 2 - Entr 1 (2)'!$G$2</c:f>
+              <c:f>'Exp2-Entr1(2)'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2301,7 +2297,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Exp 2 - Entr 1 (2)'!$F$3:$F$9</c:f>
+              <c:f>'Exp2-Entr1(2)'!$F$3:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2331,7 +2327,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Exp 2 - Entr 1 (2)'!$G$3:$G$9</c:f>
+              <c:f>'Exp2-Entr1(2)'!$G$3:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2366,7 +2362,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Exp 2 - Entr 1 (2)'!$H$2</c:f>
+              <c:f>'Exp2-Entr1(2)'!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2401,7 +2397,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Exp 2 - Entr 1 (2)'!$F$3:$F$9</c:f>
+              <c:f>'Exp2-Entr1(2)'!$F$3:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2431,7 +2427,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Exp 2 - Entr 1 (2)'!$H$3:$H$9</c:f>
+              <c:f>'Exp2-Entr1(2)'!$H$3:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2469,11 +2465,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-837433808"/>
-        <c:axId val="-892112960"/>
+        <c:axId val="-892316208"/>
+        <c:axId val="-896722336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-837433808"/>
+        <c:axId val="-892316208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2505,7 +2501,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2572,12 +2567,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-892112960"/>
+        <c:crossAx val="-896722336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-892112960"/>
+        <c:axId val="-896722336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2623,7 +2618,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2683,7 +2677,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-837433808"/>
+        <c:crossAx val="-892316208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2697,7 +2691,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2804,7 +2797,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2845,7 +2837,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Exp 2 - Entr 1 (2)'!$G$2</c:f>
+              <c:f>'Exp2-Entr1(2)'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2880,7 +2872,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Exp 2 - Entr 1 (2)'!$F$24:$F$35</c:f>
+              <c:f>'Exp2-Entr1(2)'!$F$24:$F$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2925,7 +2917,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Exp 2 - Entr 1 (2)'!$G$24:$G$35</c:f>
+              <c:f>'Exp2-Entr1(2)'!$G$24:$G$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2975,7 +2967,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Exp 2 - Entr 1 (2)'!$H$2</c:f>
+              <c:f>'Exp2-Entr1(2)'!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3010,7 +3002,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Exp 2 - Entr 1 (2)'!$F$24:$F$35</c:f>
+              <c:f>'Exp2-Entr1(2)'!$F$24:$F$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3055,7 +3047,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Exp 2 - Entr 1 (2)'!$H$24:$H$35</c:f>
+              <c:f>'Exp2-Entr1(2)'!$H$24:$H$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3108,11 +3100,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-892257296"/>
-        <c:axId val="-892255520"/>
+        <c:axId val="-931014000"/>
+        <c:axId val="-931010880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-892257296"/>
+        <c:axId val="-931014000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3144,7 +3136,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3211,12 +3202,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-892255520"/>
+        <c:crossAx val="-931010880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-892255520"/>
+        <c:axId val="-931010880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3262,7 +3253,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3322,7 +3312,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-892257296"/>
+        <c:crossAx val="-931014000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3336,7 +3326,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3366,6 +3355,480 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Tiempo Medio de Respuesta</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Exp2-Entr2'!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>900.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>800.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>700.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Exp2-Entr2'!$C$3:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>56012.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46232.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42384.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45934.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41143.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>47429.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>47283.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42649.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35609.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16911.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-930761744"/>
+        <c:axId val="-930759040"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-930761744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-930759040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-930759040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>t (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-930761744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3643,6 +4106,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -6720,6 +7223,522 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -6940,6 +7959,43 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -8303,8 +9359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:E18"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8522,7 +9578,7 @@
   <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9401,10 +10457,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C15"/>
+  <dimension ref="B2:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9419,70 +10475,86 @@
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="2">
-        <v>1300</v>
+        <v>1000</v>
+      </c>
+      <c r="C3">
+        <v>56012</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4">
-        <v>1200</v>
+        <v>900</v>
+      </c>
+      <c r="C4">
+        <v>46232</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5">
-        <v>1100</v>
+      <c r="B5" s="2">
+        <v>800</v>
+      </c>
+      <c r="C5">
+        <v>42384</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="2">
-        <v>1000</v>
+      <c r="B6">
+        <v>700</v>
+      </c>
+      <c r="C6">
+        <v>45934</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7">
-        <v>900</v>
+      <c r="B7" s="2">
+        <v>600</v>
+      </c>
+      <c r="C7">
+        <v>41143</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="2">
-        <v>800</v>
+      <c r="B8">
+        <v>500</v>
+      </c>
+      <c r="C8">
+        <v>47429</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B9">
-        <v>700</v>
+      <c r="B9" s="2">
+        <v>400</v>
+      </c>
+      <c r="C9">
+        <v>47283</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="2">
-        <v>600</v>
+      <c r="B10">
+        <v>300</v>
+      </c>
+      <c r="C10">
+        <v>42649</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B11">
-        <v>500</v>
+      <c r="B11" s="2">
+        <v>200</v>
+      </c>
+      <c r="C11">
+        <v>35609</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B12" s="2">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B13">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B15">
+      <c r="B12">
         <v>100</v>
+      </c>
+      <c r="C12">
+        <v>16911</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
grafica del exp 2.2
</commit_message>
<xml_diff>
--- a/JMeter/Experimentos.xlsx
+++ b/JMeter/Experimentos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiansanchez/IngenieriaSistemas/2017-1/ArquiSoft/Proyecto/musical-octo-happiness/JMeter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/santiago/Documents/arquisoft/musical-octo-happiness/JMeter/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="460" windowWidth="22480" windowHeight="14180" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Exp1-Entr1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="18">
   <si>
     <t>agregarMedicion</t>
   </si>
@@ -69,6 +69,21 @@
   </si>
   <si>
     <t>1 ITERACIÓN</t>
+  </si>
+  <si>
+    <t>Nodo con seguridad</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Con seguridad</t>
+  </si>
+  <si>
+    <t>Sin seguridad</t>
+  </si>
+  <si>
+    <t>Gráfico</t>
   </si>
 </sst>
 </file>
@@ -140,12 +155,76 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -168,7 +247,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -181,6 +260,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -419,11 +512,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-893104848"/>
-        <c:axId val="-893108512"/>
+        <c:axId val="-1399916944"/>
+        <c:axId val="-1435360016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-893104848"/>
+        <c:axId val="-1399916944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1200.0"/>
@@ -536,12 +629,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-893108512"/>
+        <c:crossAx val="-1435360016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-893108512"/>
+        <c:axId val="-1435360016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1200.0"/>
@@ -618,6 +711,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -654,7 +748,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-893104848"/>
+        <c:crossAx val="-1399916944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -912,11 +1006,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-837760240"/>
-        <c:axId val="-837757120"/>
+        <c:axId val="-1399901408"/>
+        <c:axId val="-1399897648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-837760240"/>
+        <c:axId val="-1399901408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1029,12 +1123,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-837757120"/>
+        <c:crossAx val="-1399897648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-837757120"/>
+        <c:axId val="-1399897648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1146,7 +1240,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-837760240"/>
+        <c:crossAx val="-1399901408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1408,11 +1502,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-837165184"/>
-        <c:axId val="-892310176"/>
+        <c:axId val="-1399871312"/>
+        <c:axId val="-1399867552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-837165184"/>
+        <c:axId val="-1399871312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1524,12 +1618,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-892310176"/>
+        <c:crossAx val="-1399867552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-892310176"/>
+        <c:axId val="-1399867552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1641,7 +1735,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-837165184"/>
+        <c:crossAx val="-1399871312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1900,11 +1994,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-837440336"/>
-        <c:axId val="-837437216"/>
+        <c:axId val="-1356832800"/>
+        <c:axId val="-1356829040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-837440336"/>
+        <c:axId val="-1356832800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2016,12 +2110,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-837437216"/>
+        <c:crossAx val="-1356829040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-837437216"/>
+        <c:axId val="-1356829040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2133,7 +2227,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-837440336"/>
+        <c:crossAx val="-1356832800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2222,6 +2316,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2465,11 +2560,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-892316208"/>
-        <c:axId val="-896722336"/>
+        <c:axId val="-1356795376"/>
+        <c:axId val="-1356791616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-892316208"/>
+        <c:axId val="-1356795376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2501,6 +2596,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2567,12 +2663,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-896722336"/>
+        <c:crossAx val="-1356791616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-896722336"/>
+        <c:axId val="-1356791616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2618,6 +2714,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2677,7 +2774,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-892316208"/>
+        <c:crossAx val="-1356795376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2691,6 +2788,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2797,6 +2895,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3100,11 +3199,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-931014000"/>
-        <c:axId val="-931010880"/>
+        <c:axId val="-1356762880"/>
+        <c:axId val="-1356759120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-931014000"/>
+        <c:axId val="-1356762880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3136,6 +3235,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3202,12 +3302,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-931010880"/>
+        <c:crossAx val="-1356759120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-931010880"/>
+        <c:axId val="-1356759120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3253,6 +3353,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3312,7 +3413,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-931014000"/>
+        <c:crossAx val="-1356762880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3326,6 +3427,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3406,63 +3508,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Tiempo Medio de Respuesta</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -3471,6 +3517,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Exp2-Entr2'!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Con seguridad</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -3495,9 +3552,23 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Exp2-Entr2'!$B$3:$B$12</c:f>
+              <c:f>'Exp2-Entr2'!$F$3:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3536,7 +3607,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Exp2-Entr2'!$C$3:$C$12</c:f>
+              <c:f>'Exp2-Entr2'!$G$3:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3569,6 +3640,138 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>16911.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Exp2-Entr2'!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sin seguridad</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Exp2-Entr2'!$F$3:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>900.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>800.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>700.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Exp2-Entr2'!$H$3:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>955.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>942.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>841.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>696.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>243.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>166.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3583,11 +3786,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-930761744"/>
-        <c:axId val="-930759040"/>
+        <c:axId val="-1331007824"/>
+        <c:axId val="-1330979856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-930761744"/>
+        <c:axId val="-1331007824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3607,6 +3810,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -3628,8 +3845,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t># Threads</a:t>
+                  <a:t>Numero</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> de threads</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -3663,8 +3885,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -3700,14 +3921,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-930759040"/>
+        <c:crossAx val="-1330979856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-930759040"/>
+        <c:axId val="-1330979856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3725,6 +3947,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -3746,7 +3982,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>t (ms)</a:t>
+                  <a:t>Media (ms)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3781,7 +4017,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -3817,7 +4053,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-930761744"/>
+        <c:crossAx val="-1331007824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3829,6 +4065,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -7963,23 +8231,21 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -9359,8 +9625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9577,8 +9843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10457,104 +10723,511 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C12"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="162" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="F1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
+        <v>1200</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="19">
+        <v>1000</v>
+      </c>
+      <c r="G3" s="11">
+        <v>56012</v>
+      </c>
+      <c r="H3" s="20">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
+        <v>1100</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="10">
+        <v>900</v>
+      </c>
+      <c r="G4" s="11">
+        <v>46232</v>
+      </c>
+      <c r="H4" s="20">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="10">
+        <v>1000</v>
+      </c>
+      <c r="B5">
+        <v>56012</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="19">
+        <v>800</v>
+      </c>
+      <c r="G5" s="11">
+        <v>42384</v>
+      </c>
+      <c r="H5" s="20">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="10">
+        <v>900</v>
+      </c>
+      <c r="B6">
+        <v>46232</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="10">
+        <v>700</v>
+      </c>
+      <c r="G6" s="11">
+        <v>45934</v>
+      </c>
+      <c r="H6" s="20">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="10">
+        <v>800</v>
+      </c>
+      <c r="B7">
+        <v>42384</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="19">
+        <v>600</v>
+      </c>
+      <c r="G7" s="11">
+        <v>41143</v>
+      </c>
+      <c r="H7" s="20">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="10">
+        <v>700</v>
+      </c>
+      <c r="B8">
+        <v>45934</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="10">
+        <v>500</v>
+      </c>
+      <c r="G8" s="11">
+        <v>47429</v>
+      </c>
+      <c r="H8" s="20">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
+        <v>600</v>
+      </c>
+      <c r="B9">
+        <v>41143</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="19">
+        <v>400</v>
+      </c>
+      <c r="G9" s="11">
+        <v>47283</v>
+      </c>
+      <c r="H9" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="10">
+        <v>500</v>
+      </c>
+      <c r="B10">
+        <v>47429</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="10">
+        <v>300</v>
+      </c>
+      <c r="G10" s="11">
+        <v>42649</v>
+      </c>
+      <c r="H10" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
+        <v>400</v>
+      </c>
+      <c r="B11">
+        <v>47283</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="19">
+        <v>200</v>
+      </c>
+      <c r="G11" s="11">
+        <v>35609</v>
+      </c>
+      <c r="H11" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="10">
+        <v>300</v>
+      </c>
+      <c r="B12">
+        <v>42649</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="13">
+        <v>100</v>
+      </c>
+      <c r="G12" s="14">
+        <v>16911</v>
+      </c>
+      <c r="H12" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="10">
+        <v>200</v>
+      </c>
+      <c r="B13">
+        <v>35609</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="13">
+        <v>100</v>
+      </c>
+      <c r="B14">
+        <v>16911</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="2">
+      <c r="C16" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="10">
+        <v>1200</v>
+      </c>
+      <c r="B17" s="11">
+        <v>1169</v>
+      </c>
+      <c r="C17" s="11">
+        <v>0</v>
+      </c>
+      <c r="D17" s="12">
+        <v>305.49898167006103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="10">
+        <v>1100</v>
+      </c>
+      <c r="B18" s="11">
+        <v>984</v>
+      </c>
+      <c r="C18" s="11">
+        <v>0</v>
+      </c>
+      <c r="D18" s="12">
+        <v>289.32140978432398</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
         <v>1000</v>
       </c>
-      <c r="C3">
-        <v>56012</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4">
+      <c r="B19" s="11">
+        <v>955</v>
+      </c>
+      <c r="C19" s="11">
+        <v>0</v>
+      </c>
+      <c r="D19" s="12">
+        <v>286.61507595299503</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="10">
         <v>900</v>
       </c>
-      <c r="C4">
-        <v>46232</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="2">
+      <c r="B20" s="11">
+        <v>942</v>
+      </c>
+      <c r="C20" s="11">
+        <v>0</v>
+      </c>
+      <c r="D20" s="12">
+        <v>284.270372710044</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="10">
         <v>800</v>
       </c>
-      <c r="C5">
-        <v>42384</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6">
+      <c r="B21" s="11">
+        <v>841</v>
+      </c>
+      <c r="C21" s="11">
+        <v>0</v>
+      </c>
+      <c r="D21" s="12">
+        <v>290.06526468455399</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="10">
         <v>700</v>
       </c>
-      <c r="C6">
-        <v>45934</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="2">
+      <c r="B22" s="11">
+        <v>696</v>
+      </c>
+      <c r="C22" s="11">
+        <v>0</v>
+      </c>
+      <c r="D22" s="12">
+        <v>297.99914857386102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="10">
         <v>600</v>
       </c>
-      <c r="C7">
-        <v>41143</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B8">
+      <c r="B23" s="11">
+        <v>243</v>
+      </c>
+      <c r="C23" s="11">
+        <v>0</v>
+      </c>
+      <c r="D23" s="12">
+        <v>308.64197530864197</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="10">
         <v>500</v>
       </c>
-      <c r="C8">
-        <v>47429</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="2">
+      <c r="B24" s="11">
+        <v>166</v>
+      </c>
+      <c r="C24" s="11">
+        <v>0</v>
+      </c>
+      <c r="D24" s="12">
+        <v>318.06615776081401</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="10">
         <v>400</v>
       </c>
-      <c r="C9">
-        <v>47283</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B10">
+      <c r="B25" s="11">
+        <v>2</v>
+      </c>
+      <c r="C25" s="11">
+        <v>0</v>
+      </c>
+      <c r="D25" s="12">
+        <v>266.31158455392801</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="10">
         <v>300</v>
       </c>
-      <c r="C10">
-        <v>42649</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="2">
+      <c r="B26" s="11">
+        <v>3</v>
+      </c>
+      <c r="C26" s="11">
+        <v>0</v>
+      </c>
+      <c r="D26" s="12">
+        <v>294.11764705882302</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="10">
         <v>200</v>
       </c>
-      <c r="C11">
-        <v>35609</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B12">
+      <c r="B27" s="11">
+        <v>2</v>
+      </c>
+      <c r="C27" s="11">
+        <v>0</v>
+      </c>
+      <c r="D27" s="12">
+        <v>173.91304347825999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="13">
         <v>100</v>
       </c>
-      <c r="C12">
-        <v>16911</v>
+      <c r="B28" s="14">
+        <v>3</v>
+      </c>
+      <c r="C28" s="14">
+        <v>0</v>
+      </c>
+      <c r="D28" s="15">
+        <v>87.796312554872699</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>